<commit_message>
Refactor in excelTestCasesTestPackPharmacyReports_SNCH.xlsx and excelTestCasesTestPackPharmacyReports_RTM.xlsx removed BillWiseSalesReport
</commit_message>
<xml_diff>
--- a/Library/excelTestCasesTestPackPharmacyReports_RTM.xlsx
+++ b/Library/excelTestCasesTestPackPharmacyReports_RTM.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QA\Automation\AutomationTest\Library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Automation\AutomationTest\Library\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28200" yWindow="0" windowWidth="13908" windowHeight="12300"/>
+    <workbookView xWindow="28200" yWindow="0" windowWidth="13905" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="test" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -39,9 +39,6 @@
     <t>TC001</t>
   </si>
   <si>
-    <t>TC004</t>
-  </si>
-  <si>
     <t>TC005</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
   </si>
   <si>
     <t>Pharmacy\Reports\Purchase\TC02PurchaseSummaryReport.py</t>
-  </si>
-  <si>
-    <t>Pharmacy\Reports\Sales\TC01BillWiseSalesReport.py.py</t>
   </si>
   <si>
     <t>Pharmacy\Reports\Sales\TC02ItemWiseSalesReport.py</t>
@@ -465,23 +459,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.5546875" customWidth="1"/>
+    <col min="1" max="1" width="54.5703125" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.77734375" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -492,7 +486,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -501,18 +495,18 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2" s="3">
         <v>0</v>
@@ -523,34 +517,34 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="3">
         <v>0</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4" s="3">
         <v>0</v>
@@ -561,15 +555,15 @@
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3">
         <v>0</v>
@@ -579,16 +573,19 @@
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="3">
         <v>0</v>
@@ -598,19 +595,16 @@
       </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="I6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3">
         <v>0</v>
@@ -621,15 +615,15 @@
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3">
         <v>0</v>
@@ -640,15 +634,15 @@
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3">
         <v>0</v>
@@ -659,15 +653,15 @@
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D10" s="3">
         <v>0</v>
@@ -677,25 +671,6 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="3">
-        <v>0</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>